<commit_message>
feat(condo): DOMA-6936 added column "Is verified" for contacts import
</commit_message>
<xml_diff>
--- a/apps/condo/public/contact-import-example-en.xlsx
+++ b/apps/condo/public/contact-import-example-en.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31">
   <si>
     <t>Address</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>Role</t>
+  </si>
+  <si>
+    <t>Is verified</t>
   </si>
   <si>
     <t xml:space="preserve"> г Арамиль, ул Гарнизон, д 19Б</t>
@@ -59,6 +62,9 @@
     <t>Resident</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>Parking place</t>
   </si>
   <si>
@@ -78,6 +84,9 @@
     <t>Owner</t>
   </si>
   <si>
+    <t>No</t>
+  </si>
+  <si>
     <t>Apartment</t>
   </si>
   <si>
@@ -106,16 +115,11 @@
         <color indexed="8"/>
         <rFont val="Calibri"/>
       </rPr>
-      <t>t</t>
+      <t>ttest@example.com</t>
     </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>test@example.com</t>
-    </r>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
   <si>
     <t>Commercial unit</t>
@@ -132,6 +136,9 @@
       </rPr>
       <t>test3@example.com</t>
     </r>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -1278,7 +1285,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1289,8 +1296,8 @@
     <col min="3" max="3" width="17.6719" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.6719" style="1" customWidth="1"/>
     <col min="5" max="5" width="40.6719" style="1" customWidth="1"/>
-    <col min="6" max="7" width="17.6719" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.5" style="1" customWidth="1"/>
+    <col min="6" max="8" width="17.6719" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.35" customHeight="1">
@@ -1315,120 +1322,136 @@
       <c r="G1" t="s" s="2">
         <v>6</v>
       </c>
+      <c r="H1" t="s" s="2">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" ht="15.35" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="4">
         <v>2</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s" s="5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s" s="5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H2" t="s" s="2">
+        <v>14</v>
       </c>
     </row>
     <row r="3" ht="15.35" customHeight="1">
       <c r="A3" t="s" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="4">
         <v>3</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s" s="5">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s" s="5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s" s="2">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s" s="2">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="H3" t="s" s="2">
+        <v>19</v>
       </c>
     </row>
     <row r="4" ht="15.35" customHeight="1">
       <c r="A4" t="s" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="4">
         <v>7</v>
       </c>
       <c r="C4" t="s" s="2">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s" s="5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s" s="5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F4" t="s" s="2">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G4" t="s" s="2">
-        <v>19</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="H4" s="2"/>
     </row>
     <row r="5" ht="15.35" customHeight="1">
       <c r="A5" t="s" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="4">
         <v>4</v>
       </c>
       <c r="C5" t="s" s="2">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s" s="5">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s" s="5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F5" t="s" s="2">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G5" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H5" t="s" s="2">
+        <v>26</v>
       </c>
     </row>
     <row r="6" ht="15.35" customHeight="1">
       <c r="A6" t="s" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" s="4">
         <v>6</v>
       </c>
       <c r="C6" t="s" s="2">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s" s="5">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s" s="5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F6" t="s" s="2">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="G6" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H6" t="s" s="2">
+        <v>30</v>
       </c>
     </row>
     <row r="7" ht="15.35" customHeight="1">
@@ -1439,6 +1462,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
     </row>
     <row r="8" ht="15.35" customHeight="1">
       <c r="A8" s="6"/>
@@ -1448,6 +1472,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
     </row>
     <row r="9" ht="15.35" customHeight="1">
       <c r="A9" s="6"/>
@@ -1457,6 +1482,7 @@
       <c r="E9" s="4"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
     </row>
     <row r="10" ht="15.35" customHeight="1">
       <c r="A10" s="6"/>
@@ -1466,6 +1492,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
     </row>
     <row r="11" ht="15.35" customHeight="1">
       <c r="A11" s="6"/>
@@ -1475,6 +1502,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
     </row>
     <row r="12" ht="15.35" customHeight="1">
       <c r="A12" s="6"/>
@@ -1484,6 +1512,7 @@
       <c r="E12" s="4"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
     </row>
     <row r="13" ht="15.35" customHeight="1">
       <c r="A13" s="6"/>
@@ -1493,6 +1522,7 @@
       <c r="E13" s="4"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
     </row>
     <row r="14" ht="15.35" customHeight="1">
       <c r="A14" s="6"/>
@@ -1502,6 +1532,7 @@
       <c r="E14" s="4"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
     </row>
     <row r="15" ht="15.35" customHeight="1">
       <c r="A15" s="6"/>
@@ -1511,6 +1542,7 @@
       <c r="E15" s="4"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
     </row>
     <row r="16" ht="15.35" customHeight="1">
       <c r="A16" s="6"/>
@@ -1520,6 +1552,7 @@
       <c r="E16" s="4"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
     </row>
     <row r="17" ht="15.35" customHeight="1">
       <c r="A17" s="6"/>
@@ -1529,6 +1562,7 @@
       <c r="E17" s="4"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
     </row>
     <row r="18" ht="15.35" customHeight="1">
       <c r="A18" s="6"/>
@@ -1538,6 +1572,7 @@
       <c r="E18" s="4"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
     </row>
     <row r="19" ht="15.35" customHeight="1">
       <c r="A19" s="6"/>
@@ -1547,6 +1582,7 @@
       <c r="E19" s="4"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
     </row>
     <row r="20" ht="15.35" customHeight="1">
       <c r="A20" s="6"/>
@@ -1556,6 +1592,7 @@
       <c r="E20" s="4"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
     </row>
     <row r="21" ht="15.35" customHeight="1">
       <c r="A21" s="6"/>
@@ -1565,6 +1602,7 @@
       <c r="E21" s="4"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
     </row>
     <row r="22" ht="15.35" customHeight="1">
       <c r="A22" s="6"/>
@@ -1574,6 +1612,7 @@
       <c r="E22" s="4"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
     </row>
     <row r="23" ht="15.35" customHeight="1">
       <c r="A23" s="6"/>
@@ -1583,6 +1622,7 @@
       <c r="E23" s="4"/>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
     </row>
     <row r="24" ht="15.35" customHeight="1">
       <c r="A24" s="6"/>
@@ -1592,6 +1632,7 @@
       <c r="E24" s="4"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
     </row>
     <row r="25" ht="15.35" customHeight="1">
       <c r="A25" s="6"/>
@@ -1601,6 +1642,7 @@
       <c r="E25" s="4"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
     </row>
     <row r="26" ht="15.35" customHeight="1">
       <c r="A26" s="6"/>
@@ -1610,6 +1652,7 @@
       <c r="E26" s="4"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
     </row>
     <row r="27" ht="15.35" customHeight="1">
       <c r="A27" s="6"/>
@@ -1619,6 +1662,7 @@
       <c r="E27" s="4"/>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
     </row>
     <row r="28" ht="15.35" customHeight="1">
       <c r="A28" s="6"/>
@@ -1628,6 +1672,7 @@
       <c r="E28" s="4"/>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
     </row>
     <row r="29" ht="15.35" customHeight="1">
       <c r="A29" s="6"/>
@@ -1637,6 +1682,7 @@
       <c r="E29" s="4"/>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
     </row>
     <row r="30" ht="15.35" customHeight="1">
       <c r="A30" s="6"/>
@@ -1646,6 +1692,7 @@
       <c r="E30" s="4"/>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
     </row>
     <row r="31" ht="15.35" customHeight="1">
       <c r="A31" s="6"/>
@@ -1655,6 +1702,7 @@
       <c r="E31" s="4"/>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
     </row>
     <row r="32" ht="15.35" customHeight="1">
       <c r="A32" s="6"/>
@@ -1664,6 +1712,7 @@
       <c r="E32" s="4"/>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
     </row>
     <row r="33" ht="15.35" customHeight="1">
       <c r="A33" s="6"/>
@@ -1673,6 +1722,7 @@
       <c r="E33" s="4"/>
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
     </row>
     <row r="34" ht="15.35" customHeight="1">
       <c r="A34" s="6"/>
@@ -1682,6 +1732,7 @@
       <c r="E34" s="4"/>
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
     </row>
     <row r="35" ht="15.35" customHeight="1">
       <c r="A35" s="6"/>
@@ -1691,6 +1742,7 @@
       <c r="E35" s="4"/>
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
     </row>
     <row r="36" ht="15.35" customHeight="1">
       <c r="A36" s="6"/>
@@ -1700,6 +1752,7 @@
       <c r="E36" s="4"/>
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
     </row>
     <row r="37" ht="15.35" customHeight="1">
       <c r="A37" s="6"/>
@@ -1709,6 +1762,7 @@
       <c r="E37" s="4"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
     </row>
     <row r="38" ht="15.35" customHeight="1">
       <c r="A38" s="6"/>
@@ -1718,6 +1772,7 @@
       <c r="E38" s="4"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
     </row>
     <row r="39" ht="15.35" customHeight="1">
       <c r="A39" s="6"/>
@@ -1727,6 +1782,7 @@
       <c r="E39" s="4"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
     </row>
     <row r="40" ht="15.35" customHeight="1">
       <c r="A40" s="6"/>
@@ -1736,6 +1792,7 @@
       <c r="E40" s="4"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
     </row>
     <row r="41" ht="15.35" customHeight="1">
       <c r="A41" s="6"/>
@@ -1745,6 +1802,7 @@
       <c r="E41" s="4"/>
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
     </row>
     <row r="42" ht="15.35" customHeight="1">
       <c r="A42" s="6"/>
@@ -1754,6 +1812,7 @@
       <c r="E42" s="4"/>
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
     </row>
     <row r="43" ht="15.35" customHeight="1">
       <c r="A43" s="6"/>
@@ -1763,6 +1822,7 @@
       <c r="E43" s="4"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
     </row>
     <row r="44" ht="15.35" customHeight="1">
       <c r="A44" s="6"/>
@@ -1772,6 +1832,7 @@
       <c r="E44" s="4"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
     </row>
     <row r="45" ht="15.35" customHeight="1">
       <c r="A45" s="6"/>
@@ -1781,6 +1842,7 @@
       <c r="E45" s="4"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
     </row>
     <row r="46" ht="15.35" customHeight="1">
       <c r="A46" s="6"/>
@@ -1790,6 +1852,7 @@
       <c r="E46" s="4"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
     </row>
     <row r="47" ht="15.35" customHeight="1">
       <c r="A47" s="6"/>
@@ -1799,6 +1862,7 @@
       <c r="E47" s="4"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
     </row>
     <row r="48" ht="15.35" customHeight="1">
       <c r="A48" s="6"/>
@@ -1808,6 +1872,7 @@
       <c r="E48" s="4"/>
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
     </row>
     <row r="49" ht="15.35" customHeight="1">
       <c r="A49" s="6"/>
@@ -1817,6 +1882,7 @@
       <c r="E49" s="4"/>
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
     </row>
     <row r="50" ht="15.35" customHeight="1">
       <c r="A50" s="6"/>
@@ -1826,13 +1892,14 @@
       <c r="E50" s="4"/>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
+      <c r="H50" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" location="" tooltip="" display="test@example.com"/>
     <hyperlink ref="F3" r:id="rId2" location="" tooltip="" display="test1@example.com"/>
     <hyperlink ref="F4" r:id="rId3" location="" tooltip="" display="test2@example.com"/>
-    <hyperlink ref="F5" r:id="rId4" location="" tooltip="" display="test@example.com"/>
+    <hyperlink ref="F5" r:id="rId4" location="" tooltip="" display="ttest@example.com"/>
     <hyperlink ref="F6" r:id="rId5" location="" tooltip="" display="test3@example.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511806" footer="0.511806"/>

</xml_diff>

<commit_message>
feat(condo): DOMA-6936 added column "Is verified" for contacts import (#3780)
</commit_message>
<xml_diff>
--- a/apps/condo/public/contact-import-example-en.xlsx
+++ b/apps/condo/public/contact-import-example-en.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31">
   <si>
     <t>Address</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>Role</t>
+  </si>
+  <si>
+    <t>Is verified</t>
   </si>
   <si>
     <t xml:space="preserve"> г Арамиль, ул Гарнизон, д 19Б</t>
@@ -59,6 +62,9 @@
     <t>Resident</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>Parking place</t>
   </si>
   <si>
@@ -78,6 +84,9 @@
     <t>Owner</t>
   </si>
   <si>
+    <t>No</t>
+  </si>
+  <si>
     <t>Apartment</t>
   </si>
   <si>
@@ -106,16 +115,11 @@
         <color indexed="8"/>
         <rFont val="Calibri"/>
       </rPr>
-      <t>t</t>
+      <t>ttest@example.com</t>
     </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>test@example.com</t>
-    </r>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
   <si>
     <t>Commercial unit</t>
@@ -132,6 +136,9 @@
       </rPr>
       <t>test3@example.com</t>
     </r>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -1278,7 +1285,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1289,8 +1296,8 @@
     <col min="3" max="3" width="17.6719" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.6719" style="1" customWidth="1"/>
     <col min="5" max="5" width="40.6719" style="1" customWidth="1"/>
-    <col min="6" max="7" width="17.6719" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.5" style="1" customWidth="1"/>
+    <col min="6" max="8" width="17.6719" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.35" customHeight="1">
@@ -1315,120 +1322,136 @@
       <c r="G1" t="s" s="2">
         <v>6</v>
       </c>
+      <c r="H1" t="s" s="2">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" ht="15.35" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="4">
         <v>2</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s" s="5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s" s="5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H2" t="s" s="2">
+        <v>14</v>
       </c>
     </row>
     <row r="3" ht="15.35" customHeight="1">
       <c r="A3" t="s" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="4">
         <v>3</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s" s="5">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s" s="5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s" s="2">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s" s="2">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="H3" t="s" s="2">
+        <v>19</v>
       </c>
     </row>
     <row r="4" ht="15.35" customHeight="1">
       <c r="A4" t="s" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="4">
         <v>7</v>
       </c>
       <c r="C4" t="s" s="2">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s" s="5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s" s="5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F4" t="s" s="2">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G4" t="s" s="2">
-        <v>19</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="H4" s="2"/>
     </row>
     <row r="5" ht="15.35" customHeight="1">
       <c r="A5" t="s" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="4">
         <v>4</v>
       </c>
       <c r="C5" t="s" s="2">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s" s="5">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s" s="5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F5" t="s" s="2">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G5" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H5" t="s" s="2">
+        <v>26</v>
       </c>
     </row>
     <row r="6" ht="15.35" customHeight="1">
       <c r="A6" t="s" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" s="4">
         <v>6</v>
       </c>
       <c r="C6" t="s" s="2">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s" s="5">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s" s="5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F6" t="s" s="2">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="G6" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H6" t="s" s="2">
+        <v>30</v>
       </c>
     </row>
     <row r="7" ht="15.35" customHeight="1">
@@ -1439,6 +1462,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
     </row>
     <row r="8" ht="15.35" customHeight="1">
       <c r="A8" s="6"/>
@@ -1448,6 +1472,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
     </row>
     <row r="9" ht="15.35" customHeight="1">
       <c r="A9" s="6"/>
@@ -1457,6 +1482,7 @@
       <c r="E9" s="4"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
     </row>
     <row r="10" ht="15.35" customHeight="1">
       <c r="A10" s="6"/>
@@ -1466,6 +1492,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
     </row>
     <row r="11" ht="15.35" customHeight="1">
       <c r="A11" s="6"/>
@@ -1475,6 +1502,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
     </row>
     <row r="12" ht="15.35" customHeight="1">
       <c r="A12" s="6"/>
@@ -1484,6 +1512,7 @@
       <c r="E12" s="4"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
     </row>
     <row r="13" ht="15.35" customHeight="1">
       <c r="A13" s="6"/>
@@ -1493,6 +1522,7 @@
       <c r="E13" s="4"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
     </row>
     <row r="14" ht="15.35" customHeight="1">
       <c r="A14" s="6"/>
@@ -1502,6 +1532,7 @@
       <c r="E14" s="4"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
     </row>
     <row r="15" ht="15.35" customHeight="1">
       <c r="A15" s="6"/>
@@ -1511,6 +1542,7 @@
       <c r="E15" s="4"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
     </row>
     <row r="16" ht="15.35" customHeight="1">
       <c r="A16" s="6"/>
@@ -1520,6 +1552,7 @@
       <c r="E16" s="4"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
     </row>
     <row r="17" ht="15.35" customHeight="1">
       <c r="A17" s="6"/>
@@ -1529,6 +1562,7 @@
       <c r="E17" s="4"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
     </row>
     <row r="18" ht="15.35" customHeight="1">
       <c r="A18" s="6"/>
@@ -1538,6 +1572,7 @@
       <c r="E18" s="4"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
     </row>
     <row r="19" ht="15.35" customHeight="1">
       <c r="A19" s="6"/>
@@ -1547,6 +1582,7 @@
       <c r="E19" s="4"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
     </row>
     <row r="20" ht="15.35" customHeight="1">
       <c r="A20" s="6"/>
@@ -1556,6 +1592,7 @@
       <c r="E20" s="4"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
     </row>
     <row r="21" ht="15.35" customHeight="1">
       <c r="A21" s="6"/>
@@ -1565,6 +1602,7 @@
       <c r="E21" s="4"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
     </row>
     <row r="22" ht="15.35" customHeight="1">
       <c r="A22" s="6"/>
@@ -1574,6 +1612,7 @@
       <c r="E22" s="4"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
     </row>
     <row r="23" ht="15.35" customHeight="1">
       <c r="A23" s="6"/>
@@ -1583,6 +1622,7 @@
       <c r="E23" s="4"/>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
     </row>
     <row r="24" ht="15.35" customHeight="1">
       <c r="A24" s="6"/>
@@ -1592,6 +1632,7 @@
       <c r="E24" s="4"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
     </row>
     <row r="25" ht="15.35" customHeight="1">
       <c r="A25" s="6"/>
@@ -1601,6 +1642,7 @@
       <c r="E25" s="4"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
     </row>
     <row r="26" ht="15.35" customHeight="1">
       <c r="A26" s="6"/>
@@ -1610,6 +1652,7 @@
       <c r="E26" s="4"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
     </row>
     <row r="27" ht="15.35" customHeight="1">
       <c r="A27" s="6"/>
@@ -1619,6 +1662,7 @@
       <c r="E27" s="4"/>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
     </row>
     <row r="28" ht="15.35" customHeight="1">
       <c r="A28" s="6"/>
@@ -1628,6 +1672,7 @@
       <c r="E28" s="4"/>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
     </row>
     <row r="29" ht="15.35" customHeight="1">
       <c r="A29" s="6"/>
@@ -1637,6 +1682,7 @@
       <c r="E29" s="4"/>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
     </row>
     <row r="30" ht="15.35" customHeight="1">
       <c r="A30" s="6"/>
@@ -1646,6 +1692,7 @@
       <c r="E30" s="4"/>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
     </row>
     <row r="31" ht="15.35" customHeight="1">
       <c r="A31" s="6"/>
@@ -1655,6 +1702,7 @@
       <c r="E31" s="4"/>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
     </row>
     <row r="32" ht="15.35" customHeight="1">
       <c r="A32" s="6"/>
@@ -1664,6 +1712,7 @@
       <c r="E32" s="4"/>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
     </row>
     <row r="33" ht="15.35" customHeight="1">
       <c r="A33" s="6"/>
@@ -1673,6 +1722,7 @@
       <c r="E33" s="4"/>
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
     </row>
     <row r="34" ht="15.35" customHeight="1">
       <c r="A34" s="6"/>
@@ -1682,6 +1732,7 @@
       <c r="E34" s="4"/>
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
     </row>
     <row r="35" ht="15.35" customHeight="1">
       <c r="A35" s="6"/>
@@ -1691,6 +1742,7 @@
       <c r="E35" s="4"/>
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
     </row>
     <row r="36" ht="15.35" customHeight="1">
       <c r="A36" s="6"/>
@@ -1700,6 +1752,7 @@
       <c r="E36" s="4"/>
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
     </row>
     <row r="37" ht="15.35" customHeight="1">
       <c r="A37" s="6"/>
@@ -1709,6 +1762,7 @@
       <c r="E37" s="4"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
     </row>
     <row r="38" ht="15.35" customHeight="1">
       <c r="A38" s="6"/>
@@ -1718,6 +1772,7 @@
       <c r="E38" s="4"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
     </row>
     <row r="39" ht="15.35" customHeight="1">
       <c r="A39" s="6"/>
@@ -1727,6 +1782,7 @@
       <c r="E39" s="4"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
     </row>
     <row r="40" ht="15.35" customHeight="1">
       <c r="A40" s="6"/>
@@ -1736,6 +1792,7 @@
       <c r="E40" s="4"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
     </row>
     <row r="41" ht="15.35" customHeight="1">
       <c r="A41" s="6"/>
@@ -1745,6 +1802,7 @@
       <c r="E41" s="4"/>
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
     </row>
     <row r="42" ht="15.35" customHeight="1">
       <c r="A42" s="6"/>
@@ -1754,6 +1812,7 @@
       <c r="E42" s="4"/>
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
     </row>
     <row r="43" ht="15.35" customHeight="1">
       <c r="A43" s="6"/>
@@ -1763,6 +1822,7 @@
       <c r="E43" s="4"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
     </row>
     <row r="44" ht="15.35" customHeight="1">
       <c r="A44" s="6"/>
@@ -1772,6 +1832,7 @@
       <c r="E44" s="4"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
     </row>
     <row r="45" ht="15.35" customHeight="1">
       <c r="A45" s="6"/>
@@ -1781,6 +1842,7 @@
       <c r="E45" s="4"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
     </row>
     <row r="46" ht="15.35" customHeight="1">
       <c r="A46" s="6"/>
@@ -1790,6 +1852,7 @@
       <c r="E46" s="4"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
     </row>
     <row r="47" ht="15.35" customHeight="1">
       <c r="A47" s="6"/>
@@ -1799,6 +1862,7 @@
       <c r="E47" s="4"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
     </row>
     <row r="48" ht="15.35" customHeight="1">
       <c r="A48" s="6"/>
@@ -1808,6 +1872,7 @@
       <c r="E48" s="4"/>
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
     </row>
     <row r="49" ht="15.35" customHeight="1">
       <c r="A49" s="6"/>
@@ -1817,6 +1882,7 @@
       <c r="E49" s="4"/>
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
     </row>
     <row r="50" ht="15.35" customHeight="1">
       <c r="A50" s="6"/>
@@ -1826,13 +1892,14 @@
       <c r="E50" s="4"/>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
+      <c r="H50" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" location="" tooltip="" display="test@example.com"/>
     <hyperlink ref="F3" r:id="rId2" location="" tooltip="" display="test1@example.com"/>
     <hyperlink ref="F4" r:id="rId3" location="" tooltip="" display="test2@example.com"/>
-    <hyperlink ref="F5" r:id="rId4" location="" tooltip="" display="test@example.com"/>
+    <hyperlink ref="F5" r:id="rId4" location="" tooltip="" display="ttest@example.com"/>
     <hyperlink ref="F6" r:id="rId5" location="" tooltip="" display="test3@example.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511806" footer="0.511806"/>

</xml_diff>

<commit_message>
Revert "feat(condo): DOMA-6936 added column "Is verified" for contacts import (#3780)"
This reverts commit 59ef145123fdb171efbc2635638712966b18ddb1.
</commit_message>
<xml_diff>
--- a/apps/condo/public/contact-import-example-en.xlsx
+++ b/apps/condo/public/contact-import-example-en.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
   <si>
     <t>Address</t>
   </si>
@@ -32,9 +32,6 @@
   </si>
   <si>
     <t>Role</t>
-  </si>
-  <si>
-    <t>Is verified</t>
   </si>
   <si>
     <t xml:space="preserve"> г Арамиль, ул Гарнизон, д 19Б</t>
@@ -62,9 +59,6 @@
     <t>Resident</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>Parking place</t>
   </si>
   <si>
@@ -84,9 +78,6 @@
     <t>Owner</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>Apartment</t>
   </si>
   <si>
@@ -115,11 +106,16 @@
         <color indexed="8"/>
         <rFont val="Calibri"/>
       </rPr>
-      <t>ttest@example.com</t>
+      <t>t</t>
     </r>
-  </si>
-  <si>
-    <t>yes</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>test@example.com</t>
+    </r>
   </si>
   <si>
     <t>Commercial unit</t>
@@ -136,9 +132,6 @@
       </rPr>
       <t>test3@example.com</t>
     </r>
-  </si>
-  <si>
-    <t>no</t>
   </si>
 </sst>
 </file>
@@ -1285,7 +1278,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1296,8 +1289,8 @@
     <col min="3" max="3" width="17.6719" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.6719" style="1" customWidth="1"/>
     <col min="5" max="5" width="40.6719" style="1" customWidth="1"/>
-    <col min="6" max="8" width="17.6719" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.5" style="1" customWidth="1"/>
+    <col min="6" max="7" width="17.6719" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.35" customHeight="1">
@@ -1322,136 +1315,120 @@
       <c r="G1" t="s" s="2">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="2">
-        <v>7</v>
-      </c>
     </row>
     <row r="2" ht="15.35" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="4">
         <v>2</v>
       </c>
       <c r="C2" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s" s="5">
         <v>9</v>
       </c>
-      <c r="D2" t="s" s="5">
+      <c r="E2" t="s" s="5">
         <v>10</v>
       </c>
-      <c r="E2" t="s" s="5">
+      <c r="F2" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="F2" t="s" s="2">
+      <c r="G2" t="s" s="2">
         <v>12</v>
-      </c>
-      <c r="G2" t="s" s="2">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s" s="2">
-        <v>14</v>
       </c>
     </row>
     <row r="3" ht="15.35" customHeight="1">
       <c r="A3" t="s" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="4">
         <v>3</v>
       </c>
       <c r="C3" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s" s="5">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s" s="5">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s" s="2">
         <v>15</v>
       </c>
-      <c r="D3" t="s" s="5">
+      <c r="G3" t="s" s="2">
         <v>16</v>
-      </c>
-      <c r="E3" t="s" s="5">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s" s="2">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s" s="2">
-        <v>18</v>
-      </c>
-      <c r="H3" t="s" s="2">
-        <v>19</v>
       </c>
     </row>
     <row r="4" ht="15.35" customHeight="1">
       <c r="A4" t="s" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="4">
         <v>7</v>
       </c>
       <c r="C4" t="s" s="2">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s" s="5">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s" s="5">
         <v>10</v>
       </c>
-      <c r="E4" t="s" s="5">
-        <v>11</v>
-      </c>
       <c r="F4" t="s" s="2">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G4" t="s" s="2">
-        <v>22</v>
-      </c>
-      <c r="H4" s="2"/>
+        <v>19</v>
+      </c>
     </row>
     <row r="5" ht="15.35" customHeight="1">
       <c r="A5" t="s" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="4">
         <v>4</v>
       </c>
       <c r="C5" t="s" s="2">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s" s="5">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s" s="5">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F5" t="s" s="2">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G5" t="s" s="2">
-        <v>13</v>
-      </c>
-      <c r="H5" t="s" s="2">
-        <v>26</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" ht="15.35" customHeight="1">
       <c r="A6" t="s" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="4">
         <v>6</v>
       </c>
       <c r="C6" t="s" s="2">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s" s="5">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s" s="5">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" t="s" s="2">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G6" t="s" s="2">
-        <v>13</v>
-      </c>
-      <c r="H6" t="s" s="2">
-        <v>30</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" ht="15.35" customHeight="1">
@@ -1462,7 +1439,6 @@
       <c r="E7" s="5"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
     </row>
     <row r="8" ht="15.35" customHeight="1">
       <c r="A8" s="6"/>
@@ -1472,7 +1448,6 @@
       <c r="E8" s="4"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
     </row>
     <row r="9" ht="15.35" customHeight="1">
       <c r="A9" s="6"/>
@@ -1482,7 +1457,6 @@
       <c r="E9" s="4"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
     </row>
     <row r="10" ht="15.35" customHeight="1">
       <c r="A10" s="6"/>
@@ -1492,7 +1466,6 @@
       <c r="E10" s="4"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
     </row>
     <row r="11" ht="15.35" customHeight="1">
       <c r="A11" s="6"/>
@@ -1502,7 +1475,6 @@
       <c r="E11" s="4"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
     </row>
     <row r="12" ht="15.35" customHeight="1">
       <c r="A12" s="6"/>
@@ -1512,7 +1484,6 @@
       <c r="E12" s="4"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
     </row>
     <row r="13" ht="15.35" customHeight="1">
       <c r="A13" s="6"/>
@@ -1522,7 +1493,6 @@
       <c r="E13" s="4"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
     </row>
     <row r="14" ht="15.35" customHeight="1">
       <c r="A14" s="6"/>
@@ -1532,7 +1502,6 @@
       <c r="E14" s="4"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
     </row>
     <row r="15" ht="15.35" customHeight="1">
       <c r="A15" s="6"/>
@@ -1542,7 +1511,6 @@
       <c r="E15" s="4"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
     </row>
     <row r="16" ht="15.35" customHeight="1">
       <c r="A16" s="6"/>
@@ -1552,7 +1520,6 @@
       <c r="E16" s="4"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
     </row>
     <row r="17" ht="15.35" customHeight="1">
       <c r="A17" s="6"/>
@@ -1562,7 +1529,6 @@
       <c r="E17" s="4"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
     </row>
     <row r="18" ht="15.35" customHeight="1">
       <c r="A18" s="6"/>
@@ -1572,7 +1538,6 @@
       <c r="E18" s="4"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
     </row>
     <row r="19" ht="15.35" customHeight="1">
       <c r="A19" s="6"/>
@@ -1582,7 +1547,6 @@
       <c r="E19" s="4"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
     </row>
     <row r="20" ht="15.35" customHeight="1">
       <c r="A20" s="6"/>
@@ -1592,7 +1556,6 @@
       <c r="E20" s="4"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
     </row>
     <row r="21" ht="15.35" customHeight="1">
       <c r="A21" s="6"/>
@@ -1602,7 +1565,6 @@
       <c r="E21" s="4"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
     </row>
     <row r="22" ht="15.35" customHeight="1">
       <c r="A22" s="6"/>
@@ -1612,7 +1574,6 @@
       <c r="E22" s="4"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
     </row>
     <row r="23" ht="15.35" customHeight="1">
       <c r="A23" s="6"/>
@@ -1622,7 +1583,6 @@
       <c r="E23" s="4"/>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
     </row>
     <row r="24" ht="15.35" customHeight="1">
       <c r="A24" s="6"/>
@@ -1632,7 +1592,6 @@
       <c r="E24" s="4"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
     </row>
     <row r="25" ht="15.35" customHeight="1">
       <c r="A25" s="6"/>
@@ -1642,7 +1601,6 @@
       <c r="E25" s="4"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
     </row>
     <row r="26" ht="15.35" customHeight="1">
       <c r="A26" s="6"/>
@@ -1652,7 +1610,6 @@
       <c r="E26" s="4"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
     </row>
     <row r="27" ht="15.35" customHeight="1">
       <c r="A27" s="6"/>
@@ -1662,7 +1619,6 @@
       <c r="E27" s="4"/>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
     </row>
     <row r="28" ht="15.35" customHeight="1">
       <c r="A28" s="6"/>
@@ -1672,7 +1628,6 @@
       <c r="E28" s="4"/>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
     </row>
     <row r="29" ht="15.35" customHeight="1">
       <c r="A29" s="6"/>
@@ -1682,7 +1637,6 @@
       <c r="E29" s="4"/>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
     </row>
     <row r="30" ht="15.35" customHeight="1">
       <c r="A30" s="6"/>
@@ -1692,7 +1646,6 @@
       <c r="E30" s="4"/>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
     </row>
     <row r="31" ht="15.35" customHeight="1">
       <c r="A31" s="6"/>
@@ -1702,7 +1655,6 @@
       <c r="E31" s="4"/>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
     </row>
     <row r="32" ht="15.35" customHeight="1">
       <c r="A32" s="6"/>
@@ -1712,7 +1664,6 @@
       <c r="E32" s="4"/>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
     </row>
     <row r="33" ht="15.35" customHeight="1">
       <c r="A33" s="6"/>
@@ -1722,7 +1673,6 @@
       <c r="E33" s="4"/>
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
     </row>
     <row r="34" ht="15.35" customHeight="1">
       <c r="A34" s="6"/>
@@ -1732,7 +1682,6 @@
       <c r="E34" s="4"/>
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
     </row>
     <row r="35" ht="15.35" customHeight="1">
       <c r="A35" s="6"/>
@@ -1742,7 +1691,6 @@
       <c r="E35" s="4"/>
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
     </row>
     <row r="36" ht="15.35" customHeight="1">
       <c r="A36" s="6"/>
@@ -1752,7 +1700,6 @@
       <c r="E36" s="4"/>
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
     </row>
     <row r="37" ht="15.35" customHeight="1">
       <c r="A37" s="6"/>
@@ -1762,7 +1709,6 @@
       <c r="E37" s="4"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
     </row>
     <row r="38" ht="15.35" customHeight="1">
       <c r="A38" s="6"/>
@@ -1772,7 +1718,6 @@
       <c r="E38" s="4"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
     </row>
     <row r="39" ht="15.35" customHeight="1">
       <c r="A39" s="6"/>
@@ -1782,7 +1727,6 @@
       <c r="E39" s="4"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
     </row>
     <row r="40" ht="15.35" customHeight="1">
       <c r="A40" s="6"/>
@@ -1792,7 +1736,6 @@
       <c r="E40" s="4"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
     </row>
     <row r="41" ht="15.35" customHeight="1">
       <c r="A41" s="6"/>
@@ -1802,7 +1745,6 @@
       <c r="E41" s="4"/>
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
     </row>
     <row r="42" ht="15.35" customHeight="1">
       <c r="A42" s="6"/>
@@ -1812,7 +1754,6 @@
       <c r="E42" s="4"/>
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
-      <c r="H42" s="6"/>
     </row>
     <row r="43" ht="15.35" customHeight="1">
       <c r="A43" s="6"/>
@@ -1822,7 +1763,6 @@
       <c r="E43" s="4"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="6"/>
     </row>
     <row r="44" ht="15.35" customHeight="1">
       <c r="A44" s="6"/>
@@ -1832,7 +1772,6 @@
       <c r="E44" s="4"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="6"/>
     </row>
     <row r="45" ht="15.35" customHeight="1">
       <c r="A45" s="6"/>
@@ -1842,7 +1781,6 @@
       <c r="E45" s="4"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="6"/>
     </row>
     <row r="46" ht="15.35" customHeight="1">
       <c r="A46" s="6"/>
@@ -1852,7 +1790,6 @@
       <c r="E46" s="4"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="6"/>
     </row>
     <row r="47" ht="15.35" customHeight="1">
       <c r="A47" s="6"/>
@@ -1862,7 +1799,6 @@
       <c r="E47" s="4"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="6"/>
     </row>
     <row r="48" ht="15.35" customHeight="1">
       <c r="A48" s="6"/>
@@ -1872,7 +1808,6 @@
       <c r="E48" s="4"/>
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
-      <c r="H48" s="6"/>
     </row>
     <row r="49" ht="15.35" customHeight="1">
       <c r="A49" s="6"/>
@@ -1882,7 +1817,6 @@
       <c r="E49" s="4"/>
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
-      <c r="H49" s="6"/>
     </row>
     <row r="50" ht="15.35" customHeight="1">
       <c r="A50" s="6"/>
@@ -1892,14 +1826,13 @@
       <c r="E50" s="4"/>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
-      <c r="H50" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" location="" tooltip="" display="test@example.com"/>
     <hyperlink ref="F3" r:id="rId2" location="" tooltip="" display="test1@example.com"/>
     <hyperlink ref="F4" r:id="rId3" location="" tooltip="" display="test2@example.com"/>
-    <hyperlink ref="F5" r:id="rId4" location="" tooltip="" display="ttest@example.com"/>
+    <hyperlink ref="F5" r:id="rId4" location="" tooltip="" display="test@example.com"/>
     <hyperlink ref="F6" r:id="rId5" location="" tooltip="" display="test3@example.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511806" footer="0.511806"/>

</xml_diff>

<commit_message>
Revert "feat(condo): DOMA-6936 added column "Is verified" for contacts import (#3780)" (#3810)
This reverts commit 59ef145123fdb171efbc2635638712966b18ddb1.
</commit_message>
<xml_diff>
--- a/apps/condo/public/contact-import-example-en.xlsx
+++ b/apps/condo/public/contact-import-example-en.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
   <si>
     <t>Address</t>
   </si>
@@ -32,9 +32,6 @@
   </si>
   <si>
     <t>Role</t>
-  </si>
-  <si>
-    <t>Is verified</t>
   </si>
   <si>
     <t xml:space="preserve"> г Арамиль, ул Гарнизон, д 19Б</t>
@@ -62,9 +59,6 @@
     <t>Resident</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>Parking place</t>
   </si>
   <si>
@@ -84,9 +78,6 @@
     <t>Owner</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>Apartment</t>
   </si>
   <si>
@@ -115,11 +106,16 @@
         <color indexed="8"/>
         <rFont val="Calibri"/>
       </rPr>
-      <t>ttest@example.com</t>
+      <t>t</t>
     </r>
-  </si>
-  <si>
-    <t>yes</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>test@example.com</t>
+    </r>
   </si>
   <si>
     <t>Commercial unit</t>
@@ -136,9 +132,6 @@
       </rPr>
       <t>test3@example.com</t>
     </r>
-  </si>
-  <si>
-    <t>no</t>
   </si>
 </sst>
 </file>
@@ -1285,7 +1278,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1296,8 +1289,8 @@
     <col min="3" max="3" width="17.6719" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.6719" style="1" customWidth="1"/>
     <col min="5" max="5" width="40.6719" style="1" customWidth="1"/>
-    <col min="6" max="8" width="17.6719" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.5" style="1" customWidth="1"/>
+    <col min="6" max="7" width="17.6719" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.35" customHeight="1">
@@ -1322,136 +1315,120 @@
       <c r="G1" t="s" s="2">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="2">
-        <v>7</v>
-      </c>
     </row>
     <row r="2" ht="15.35" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="4">
         <v>2</v>
       </c>
       <c r="C2" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s" s="5">
         <v>9</v>
       </c>
-      <c r="D2" t="s" s="5">
+      <c r="E2" t="s" s="5">
         <v>10</v>
       </c>
-      <c r="E2" t="s" s="5">
+      <c r="F2" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="F2" t="s" s="2">
+      <c r="G2" t="s" s="2">
         <v>12</v>
-      </c>
-      <c r="G2" t="s" s="2">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s" s="2">
-        <v>14</v>
       </c>
     </row>
     <row r="3" ht="15.35" customHeight="1">
       <c r="A3" t="s" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="4">
         <v>3</v>
       </c>
       <c r="C3" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s" s="5">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s" s="5">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s" s="2">
         <v>15</v>
       </c>
-      <c r="D3" t="s" s="5">
+      <c r="G3" t="s" s="2">
         <v>16</v>
-      </c>
-      <c r="E3" t="s" s="5">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s" s="2">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s" s="2">
-        <v>18</v>
-      </c>
-      <c r="H3" t="s" s="2">
-        <v>19</v>
       </c>
     </row>
     <row r="4" ht="15.35" customHeight="1">
       <c r="A4" t="s" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="4">
         <v>7</v>
       </c>
       <c r="C4" t="s" s="2">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s" s="5">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s" s="5">
         <v>10</v>
       </c>
-      <c r="E4" t="s" s="5">
-        <v>11</v>
-      </c>
       <c r="F4" t="s" s="2">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G4" t="s" s="2">
-        <v>22</v>
-      </c>
-      <c r="H4" s="2"/>
+        <v>19</v>
+      </c>
     </row>
     <row r="5" ht="15.35" customHeight="1">
       <c r="A5" t="s" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="4">
         <v>4</v>
       </c>
       <c r="C5" t="s" s="2">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s" s="5">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s" s="5">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F5" t="s" s="2">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G5" t="s" s="2">
-        <v>13</v>
-      </c>
-      <c r="H5" t="s" s="2">
-        <v>26</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" ht="15.35" customHeight="1">
       <c r="A6" t="s" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="4">
         <v>6</v>
       </c>
       <c r="C6" t="s" s="2">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s" s="5">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s" s="5">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" t="s" s="2">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G6" t="s" s="2">
-        <v>13</v>
-      </c>
-      <c r="H6" t="s" s="2">
-        <v>30</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" ht="15.35" customHeight="1">
@@ -1462,7 +1439,6 @@
       <c r="E7" s="5"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
     </row>
     <row r="8" ht="15.35" customHeight="1">
       <c r="A8" s="6"/>
@@ -1472,7 +1448,6 @@
       <c r="E8" s="4"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
     </row>
     <row r="9" ht="15.35" customHeight="1">
       <c r="A9" s="6"/>
@@ -1482,7 +1457,6 @@
       <c r="E9" s="4"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
     </row>
     <row r="10" ht="15.35" customHeight="1">
       <c r="A10" s="6"/>
@@ -1492,7 +1466,6 @@
       <c r="E10" s="4"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
     </row>
     <row r="11" ht="15.35" customHeight="1">
       <c r="A11" s="6"/>
@@ -1502,7 +1475,6 @@
       <c r="E11" s="4"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
     </row>
     <row r="12" ht="15.35" customHeight="1">
       <c r="A12" s="6"/>
@@ -1512,7 +1484,6 @@
       <c r="E12" s="4"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
     </row>
     <row r="13" ht="15.35" customHeight="1">
       <c r="A13" s="6"/>
@@ -1522,7 +1493,6 @@
       <c r="E13" s="4"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
     </row>
     <row r="14" ht="15.35" customHeight="1">
       <c r="A14" s="6"/>
@@ -1532,7 +1502,6 @@
       <c r="E14" s="4"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
     </row>
     <row r="15" ht="15.35" customHeight="1">
       <c r="A15" s="6"/>
@@ -1542,7 +1511,6 @@
       <c r="E15" s="4"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
     </row>
     <row r="16" ht="15.35" customHeight="1">
       <c r="A16" s="6"/>
@@ -1552,7 +1520,6 @@
       <c r="E16" s="4"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
     </row>
     <row r="17" ht="15.35" customHeight="1">
       <c r="A17" s="6"/>
@@ -1562,7 +1529,6 @@
       <c r="E17" s="4"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
     </row>
     <row r="18" ht="15.35" customHeight="1">
       <c r="A18" s="6"/>
@@ -1572,7 +1538,6 @@
       <c r="E18" s="4"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
     </row>
     <row r="19" ht="15.35" customHeight="1">
       <c r="A19" s="6"/>
@@ -1582,7 +1547,6 @@
       <c r="E19" s="4"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
     </row>
     <row r="20" ht="15.35" customHeight="1">
       <c r="A20" s="6"/>
@@ -1592,7 +1556,6 @@
       <c r="E20" s="4"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
     </row>
     <row r="21" ht="15.35" customHeight="1">
       <c r="A21" s="6"/>
@@ -1602,7 +1565,6 @@
       <c r="E21" s="4"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
     </row>
     <row r="22" ht="15.35" customHeight="1">
       <c r="A22" s="6"/>
@@ -1612,7 +1574,6 @@
       <c r="E22" s="4"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
     </row>
     <row r="23" ht="15.35" customHeight="1">
       <c r="A23" s="6"/>
@@ -1622,7 +1583,6 @@
       <c r="E23" s="4"/>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
     </row>
     <row r="24" ht="15.35" customHeight="1">
       <c r="A24" s="6"/>
@@ -1632,7 +1592,6 @@
       <c r="E24" s="4"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
     </row>
     <row r="25" ht="15.35" customHeight="1">
       <c r="A25" s="6"/>
@@ -1642,7 +1601,6 @@
       <c r="E25" s="4"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
     </row>
     <row r="26" ht="15.35" customHeight="1">
       <c r="A26" s="6"/>
@@ -1652,7 +1610,6 @@
       <c r="E26" s="4"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
     </row>
     <row r="27" ht="15.35" customHeight="1">
       <c r="A27" s="6"/>
@@ -1662,7 +1619,6 @@
       <c r="E27" s="4"/>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
     </row>
     <row r="28" ht="15.35" customHeight="1">
       <c r="A28" s="6"/>
@@ -1672,7 +1628,6 @@
       <c r="E28" s="4"/>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
     </row>
     <row r="29" ht="15.35" customHeight="1">
       <c r="A29" s="6"/>
@@ -1682,7 +1637,6 @@
       <c r="E29" s="4"/>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
     </row>
     <row r="30" ht="15.35" customHeight="1">
       <c r="A30" s="6"/>
@@ -1692,7 +1646,6 @@
       <c r="E30" s="4"/>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
     </row>
     <row r="31" ht="15.35" customHeight="1">
       <c r="A31" s="6"/>
@@ -1702,7 +1655,6 @@
       <c r="E31" s="4"/>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
     </row>
     <row r="32" ht="15.35" customHeight="1">
       <c r="A32" s="6"/>
@@ -1712,7 +1664,6 @@
       <c r="E32" s="4"/>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
     </row>
     <row r="33" ht="15.35" customHeight="1">
       <c r="A33" s="6"/>
@@ -1722,7 +1673,6 @@
       <c r="E33" s="4"/>
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
     </row>
     <row r="34" ht="15.35" customHeight="1">
       <c r="A34" s="6"/>
@@ -1732,7 +1682,6 @@
       <c r="E34" s="4"/>
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
     </row>
     <row r="35" ht="15.35" customHeight="1">
       <c r="A35" s="6"/>
@@ -1742,7 +1691,6 @@
       <c r="E35" s="4"/>
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
     </row>
     <row r="36" ht="15.35" customHeight="1">
       <c r="A36" s="6"/>
@@ -1752,7 +1700,6 @@
       <c r="E36" s="4"/>
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
     </row>
     <row r="37" ht="15.35" customHeight="1">
       <c r="A37" s="6"/>
@@ -1762,7 +1709,6 @@
       <c r="E37" s="4"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
     </row>
     <row r="38" ht="15.35" customHeight="1">
       <c r="A38" s="6"/>
@@ -1772,7 +1718,6 @@
       <c r="E38" s="4"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
     </row>
     <row r="39" ht="15.35" customHeight="1">
       <c r="A39" s="6"/>
@@ -1782,7 +1727,6 @@
       <c r="E39" s="4"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
     </row>
     <row r="40" ht="15.35" customHeight="1">
       <c r="A40" s="6"/>
@@ -1792,7 +1736,6 @@
       <c r="E40" s="4"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
     </row>
     <row r="41" ht="15.35" customHeight="1">
       <c r="A41" s="6"/>
@@ -1802,7 +1745,6 @@
       <c r="E41" s="4"/>
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
     </row>
     <row r="42" ht="15.35" customHeight="1">
       <c r="A42" s="6"/>
@@ -1812,7 +1754,6 @@
       <c r="E42" s="4"/>
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
-      <c r="H42" s="6"/>
     </row>
     <row r="43" ht="15.35" customHeight="1">
       <c r="A43" s="6"/>
@@ -1822,7 +1763,6 @@
       <c r="E43" s="4"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="6"/>
     </row>
     <row r="44" ht="15.35" customHeight="1">
       <c r="A44" s="6"/>
@@ -1832,7 +1772,6 @@
       <c r="E44" s="4"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="6"/>
     </row>
     <row r="45" ht="15.35" customHeight="1">
       <c r="A45" s="6"/>
@@ -1842,7 +1781,6 @@
       <c r="E45" s="4"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="6"/>
     </row>
     <row r="46" ht="15.35" customHeight="1">
       <c r="A46" s="6"/>
@@ -1852,7 +1790,6 @@
       <c r="E46" s="4"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="6"/>
     </row>
     <row r="47" ht="15.35" customHeight="1">
       <c r="A47" s="6"/>
@@ -1862,7 +1799,6 @@
       <c r="E47" s="4"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="6"/>
     </row>
     <row r="48" ht="15.35" customHeight="1">
       <c r="A48" s="6"/>
@@ -1872,7 +1808,6 @@
       <c r="E48" s="4"/>
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
-      <c r="H48" s="6"/>
     </row>
     <row r="49" ht="15.35" customHeight="1">
       <c r="A49" s="6"/>
@@ -1882,7 +1817,6 @@
       <c r="E49" s="4"/>
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
-      <c r="H49" s="6"/>
     </row>
     <row r="50" ht="15.35" customHeight="1">
       <c r="A50" s="6"/>
@@ -1892,14 +1826,13 @@
       <c r="E50" s="4"/>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
-      <c r="H50" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" location="" tooltip="" display="test@example.com"/>
     <hyperlink ref="F3" r:id="rId2" location="" tooltip="" display="test1@example.com"/>
     <hyperlink ref="F4" r:id="rId3" location="" tooltip="" display="test2@example.com"/>
-    <hyperlink ref="F5" r:id="rId4" location="" tooltip="" display="ttest@example.com"/>
+    <hyperlink ref="F5" r:id="rId4" location="" tooltip="" display="test@example.com"/>
     <hyperlink ref="F6" r:id="rId5" location="" tooltip="" display="test3@example.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511806" footer="0.511806"/>

</xml_diff>

<commit_message>
Revert "Revert "feat(condo): DOMA-6936 added column "Is verified" for contacts import (#3780)" (#3810)"
This reverts commit 17a7e30375b4be499918538468989085488fe268.
</commit_message>
<xml_diff>
--- a/apps/condo/public/contact-import-example-en.xlsx
+++ b/apps/condo/public/contact-import-example-en.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31">
   <si>
     <t>Address</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>Role</t>
+  </si>
+  <si>
+    <t>Is verified</t>
   </si>
   <si>
     <t xml:space="preserve"> г Арамиль, ул Гарнизон, д 19Б</t>
@@ -59,6 +62,9 @@
     <t>Resident</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>Parking place</t>
   </si>
   <si>
@@ -78,6 +84,9 @@
     <t>Owner</t>
   </si>
   <si>
+    <t>No</t>
+  </si>
+  <si>
     <t>Apartment</t>
   </si>
   <si>
@@ -106,16 +115,11 @@
         <color indexed="8"/>
         <rFont val="Calibri"/>
       </rPr>
-      <t>t</t>
+      <t>ttest@example.com</t>
     </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>test@example.com</t>
-    </r>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
   <si>
     <t>Commercial unit</t>
@@ -132,6 +136,9 @@
       </rPr>
       <t>test3@example.com</t>
     </r>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -1278,7 +1285,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1289,8 +1296,8 @@
     <col min="3" max="3" width="17.6719" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.6719" style="1" customWidth="1"/>
     <col min="5" max="5" width="40.6719" style="1" customWidth="1"/>
-    <col min="6" max="7" width="17.6719" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.5" style="1" customWidth="1"/>
+    <col min="6" max="8" width="17.6719" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.35" customHeight="1">
@@ -1315,120 +1322,136 @@
       <c r="G1" t="s" s="2">
         <v>6</v>
       </c>
+      <c r="H1" t="s" s="2">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" ht="15.35" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="4">
         <v>2</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s" s="5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s" s="5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H2" t="s" s="2">
+        <v>14</v>
       </c>
     </row>
     <row r="3" ht="15.35" customHeight="1">
       <c r="A3" t="s" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="4">
         <v>3</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s" s="5">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s" s="5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s" s="2">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s" s="2">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="H3" t="s" s="2">
+        <v>19</v>
       </c>
     </row>
     <row r="4" ht="15.35" customHeight="1">
       <c r="A4" t="s" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="4">
         <v>7</v>
       </c>
       <c r="C4" t="s" s="2">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s" s="5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s" s="5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F4" t="s" s="2">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G4" t="s" s="2">
-        <v>19</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="H4" s="2"/>
     </row>
     <row r="5" ht="15.35" customHeight="1">
       <c r="A5" t="s" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="4">
         <v>4</v>
       </c>
       <c r="C5" t="s" s="2">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s" s="5">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s" s="5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F5" t="s" s="2">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G5" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H5" t="s" s="2">
+        <v>26</v>
       </c>
     </row>
     <row r="6" ht="15.35" customHeight="1">
       <c r="A6" t="s" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" s="4">
         <v>6</v>
       </c>
       <c r="C6" t="s" s="2">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s" s="5">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s" s="5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F6" t="s" s="2">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="G6" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H6" t="s" s="2">
+        <v>30</v>
       </c>
     </row>
     <row r="7" ht="15.35" customHeight="1">
@@ -1439,6 +1462,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
     </row>
     <row r="8" ht="15.35" customHeight="1">
       <c r="A8" s="6"/>
@@ -1448,6 +1472,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
     </row>
     <row r="9" ht="15.35" customHeight="1">
       <c r="A9" s="6"/>
@@ -1457,6 +1482,7 @@
       <c r="E9" s="4"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
     </row>
     <row r="10" ht="15.35" customHeight="1">
       <c r="A10" s="6"/>
@@ -1466,6 +1492,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
     </row>
     <row r="11" ht="15.35" customHeight="1">
       <c r="A11" s="6"/>
@@ -1475,6 +1502,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
     </row>
     <row r="12" ht="15.35" customHeight="1">
       <c r="A12" s="6"/>
@@ -1484,6 +1512,7 @@
       <c r="E12" s="4"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
     </row>
     <row r="13" ht="15.35" customHeight="1">
       <c r="A13" s="6"/>
@@ -1493,6 +1522,7 @@
       <c r="E13" s="4"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
     </row>
     <row r="14" ht="15.35" customHeight="1">
       <c r="A14" s="6"/>
@@ -1502,6 +1532,7 @@
       <c r="E14" s="4"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
     </row>
     <row r="15" ht="15.35" customHeight="1">
       <c r="A15" s="6"/>
@@ -1511,6 +1542,7 @@
       <c r="E15" s="4"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
     </row>
     <row r="16" ht="15.35" customHeight="1">
       <c r="A16" s="6"/>
@@ -1520,6 +1552,7 @@
       <c r="E16" s="4"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
     </row>
     <row r="17" ht="15.35" customHeight="1">
       <c r="A17" s="6"/>
@@ -1529,6 +1562,7 @@
       <c r="E17" s="4"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
     </row>
     <row r="18" ht="15.35" customHeight="1">
       <c r="A18" s="6"/>
@@ -1538,6 +1572,7 @@
       <c r="E18" s="4"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
     </row>
     <row r="19" ht="15.35" customHeight="1">
       <c r="A19" s="6"/>
@@ -1547,6 +1582,7 @@
       <c r="E19" s="4"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
     </row>
     <row r="20" ht="15.35" customHeight="1">
       <c r="A20" s="6"/>
@@ -1556,6 +1592,7 @@
       <c r="E20" s="4"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
     </row>
     <row r="21" ht="15.35" customHeight="1">
       <c r="A21" s="6"/>
@@ -1565,6 +1602,7 @@
       <c r="E21" s="4"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
     </row>
     <row r="22" ht="15.35" customHeight="1">
       <c r="A22" s="6"/>
@@ -1574,6 +1612,7 @@
       <c r="E22" s="4"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
     </row>
     <row r="23" ht="15.35" customHeight="1">
       <c r="A23" s="6"/>
@@ -1583,6 +1622,7 @@
       <c r="E23" s="4"/>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
     </row>
     <row r="24" ht="15.35" customHeight="1">
       <c r="A24" s="6"/>
@@ -1592,6 +1632,7 @@
       <c r="E24" s="4"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
     </row>
     <row r="25" ht="15.35" customHeight="1">
       <c r="A25" s="6"/>
@@ -1601,6 +1642,7 @@
       <c r="E25" s="4"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
     </row>
     <row r="26" ht="15.35" customHeight="1">
       <c r="A26" s="6"/>
@@ -1610,6 +1652,7 @@
       <c r="E26" s="4"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
     </row>
     <row r="27" ht="15.35" customHeight="1">
       <c r="A27" s="6"/>
@@ -1619,6 +1662,7 @@
       <c r="E27" s="4"/>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
     </row>
     <row r="28" ht="15.35" customHeight="1">
       <c r="A28" s="6"/>
@@ -1628,6 +1672,7 @@
       <c r="E28" s="4"/>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
     </row>
     <row r="29" ht="15.35" customHeight="1">
       <c r="A29" s="6"/>
@@ -1637,6 +1682,7 @@
       <c r="E29" s="4"/>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
     </row>
     <row r="30" ht="15.35" customHeight="1">
       <c r="A30" s="6"/>
@@ -1646,6 +1692,7 @@
       <c r="E30" s="4"/>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
     </row>
     <row r="31" ht="15.35" customHeight="1">
       <c r="A31" s="6"/>
@@ -1655,6 +1702,7 @@
       <c r="E31" s="4"/>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
     </row>
     <row r="32" ht="15.35" customHeight="1">
       <c r="A32" s="6"/>
@@ -1664,6 +1712,7 @@
       <c r="E32" s="4"/>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
     </row>
     <row r="33" ht="15.35" customHeight="1">
       <c r="A33" s="6"/>
@@ -1673,6 +1722,7 @@
       <c r="E33" s="4"/>
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
     </row>
     <row r="34" ht="15.35" customHeight="1">
       <c r="A34" s="6"/>
@@ -1682,6 +1732,7 @@
       <c r="E34" s="4"/>
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
     </row>
     <row r="35" ht="15.35" customHeight="1">
       <c r="A35" s="6"/>
@@ -1691,6 +1742,7 @@
       <c r="E35" s="4"/>
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
     </row>
     <row r="36" ht="15.35" customHeight="1">
       <c r="A36" s="6"/>
@@ -1700,6 +1752,7 @@
       <c r="E36" s="4"/>
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
     </row>
     <row r="37" ht="15.35" customHeight="1">
       <c r="A37" s="6"/>
@@ -1709,6 +1762,7 @@
       <c r="E37" s="4"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
     </row>
     <row r="38" ht="15.35" customHeight="1">
       <c r="A38" s="6"/>
@@ -1718,6 +1772,7 @@
       <c r="E38" s="4"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
     </row>
     <row r="39" ht="15.35" customHeight="1">
       <c r="A39" s="6"/>
@@ -1727,6 +1782,7 @@
       <c r="E39" s="4"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
     </row>
     <row r="40" ht="15.35" customHeight="1">
       <c r="A40" s="6"/>
@@ -1736,6 +1792,7 @@
       <c r="E40" s="4"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
     </row>
     <row r="41" ht="15.35" customHeight="1">
       <c r="A41" s="6"/>
@@ -1745,6 +1802,7 @@
       <c r="E41" s="4"/>
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
     </row>
     <row r="42" ht="15.35" customHeight="1">
       <c r="A42" s="6"/>
@@ -1754,6 +1812,7 @@
       <c r="E42" s="4"/>
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
     </row>
     <row r="43" ht="15.35" customHeight="1">
       <c r="A43" s="6"/>
@@ -1763,6 +1822,7 @@
       <c r="E43" s="4"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
     </row>
     <row r="44" ht="15.35" customHeight="1">
       <c r="A44" s="6"/>
@@ -1772,6 +1832,7 @@
       <c r="E44" s="4"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
     </row>
     <row r="45" ht="15.35" customHeight="1">
       <c r="A45" s="6"/>
@@ -1781,6 +1842,7 @@
       <c r="E45" s="4"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
     </row>
     <row r="46" ht="15.35" customHeight="1">
       <c r="A46" s="6"/>
@@ -1790,6 +1852,7 @@
       <c r="E46" s="4"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
     </row>
     <row r="47" ht="15.35" customHeight="1">
       <c r="A47" s="6"/>
@@ -1799,6 +1862,7 @@
       <c r="E47" s="4"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
     </row>
     <row r="48" ht="15.35" customHeight="1">
       <c r="A48" s="6"/>
@@ -1808,6 +1872,7 @@
       <c r="E48" s="4"/>
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
     </row>
     <row r="49" ht="15.35" customHeight="1">
       <c r="A49" s="6"/>
@@ -1817,6 +1882,7 @@
       <c r="E49" s="4"/>
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
     </row>
     <row r="50" ht="15.35" customHeight="1">
       <c r="A50" s="6"/>
@@ -1826,13 +1892,14 @@
       <c r="E50" s="4"/>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
+      <c r="H50" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" location="" tooltip="" display="test@example.com"/>
     <hyperlink ref="F3" r:id="rId2" location="" tooltip="" display="test1@example.com"/>
     <hyperlink ref="F4" r:id="rId3" location="" tooltip="" display="test2@example.com"/>
-    <hyperlink ref="F5" r:id="rId4" location="" tooltip="" display="test@example.com"/>
+    <hyperlink ref="F5" r:id="rId4" location="" tooltip="" display="ttest@example.com"/>
     <hyperlink ref="F6" r:id="rId5" location="" tooltip="" display="test3@example.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511806" footer="0.511806"/>

</xml_diff>

<commit_message>
feat(condo): DOMA-6936 added column "Is verified" for contacts import (#3865)
* Revert "Revert "feat(condo): DOMA-6936 added column "Is verified" for contacts import (#3780)" (#3810)"

This reverts commit 17a7e30375b4be499918538468989085488fe268.

* fix(condo): DOMA-6936 fixed normalizeBooleanValue
</commit_message>
<xml_diff>
--- a/apps/condo/public/contact-import-example-en.xlsx
+++ b/apps/condo/public/contact-import-example-en.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31">
   <si>
     <t>Address</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>Role</t>
+  </si>
+  <si>
+    <t>Is verified</t>
   </si>
   <si>
     <t xml:space="preserve"> г Арамиль, ул Гарнизон, д 19Б</t>
@@ -59,6 +62,9 @@
     <t>Resident</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>Parking place</t>
   </si>
   <si>
@@ -78,6 +84,9 @@
     <t>Owner</t>
   </si>
   <si>
+    <t>No</t>
+  </si>
+  <si>
     <t>Apartment</t>
   </si>
   <si>
@@ -106,16 +115,11 @@
         <color indexed="8"/>
         <rFont val="Calibri"/>
       </rPr>
-      <t>t</t>
+      <t>ttest@example.com</t>
     </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>test@example.com</t>
-    </r>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
   <si>
     <t>Commercial unit</t>
@@ -132,6 +136,9 @@
       </rPr>
       <t>test3@example.com</t>
     </r>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -1278,7 +1285,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1289,8 +1296,8 @@
     <col min="3" max="3" width="17.6719" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.6719" style="1" customWidth="1"/>
     <col min="5" max="5" width="40.6719" style="1" customWidth="1"/>
-    <col min="6" max="7" width="17.6719" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.5" style="1" customWidth="1"/>
+    <col min="6" max="8" width="17.6719" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.35" customHeight="1">
@@ -1315,120 +1322,136 @@
       <c r="G1" t="s" s="2">
         <v>6</v>
       </c>
+      <c r="H1" t="s" s="2">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" ht="15.35" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="4">
         <v>2</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s" s="5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s" s="5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H2" t="s" s="2">
+        <v>14</v>
       </c>
     </row>
     <row r="3" ht="15.35" customHeight="1">
       <c r="A3" t="s" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="4">
         <v>3</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s" s="5">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s" s="5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s" s="2">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s" s="2">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="H3" t="s" s="2">
+        <v>19</v>
       </c>
     </row>
     <row r="4" ht="15.35" customHeight="1">
       <c r="A4" t="s" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="4">
         <v>7</v>
       </c>
       <c r="C4" t="s" s="2">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s" s="5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s" s="5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F4" t="s" s="2">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G4" t="s" s="2">
-        <v>19</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="H4" s="2"/>
     </row>
     <row r="5" ht="15.35" customHeight="1">
       <c r="A5" t="s" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="4">
         <v>4</v>
       </c>
       <c r="C5" t="s" s="2">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s" s="5">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s" s="5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F5" t="s" s="2">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G5" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H5" t="s" s="2">
+        <v>26</v>
       </c>
     </row>
     <row r="6" ht="15.35" customHeight="1">
       <c r="A6" t="s" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" s="4">
         <v>6</v>
       </c>
       <c r="C6" t="s" s="2">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s" s="5">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s" s="5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F6" t="s" s="2">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="G6" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="H6" t="s" s="2">
+        <v>30</v>
       </c>
     </row>
     <row r="7" ht="15.35" customHeight="1">
@@ -1439,6 +1462,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
     </row>
     <row r="8" ht="15.35" customHeight="1">
       <c r="A8" s="6"/>
@@ -1448,6 +1472,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
     </row>
     <row r="9" ht="15.35" customHeight="1">
       <c r="A9" s="6"/>
@@ -1457,6 +1482,7 @@
       <c r="E9" s="4"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
     </row>
     <row r="10" ht="15.35" customHeight="1">
       <c r="A10" s="6"/>
@@ -1466,6 +1492,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
     </row>
     <row r="11" ht="15.35" customHeight="1">
       <c r="A11" s="6"/>
@@ -1475,6 +1502,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
     </row>
     <row r="12" ht="15.35" customHeight="1">
       <c r="A12" s="6"/>
@@ -1484,6 +1512,7 @@
       <c r="E12" s="4"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
     </row>
     <row r="13" ht="15.35" customHeight="1">
       <c r="A13" s="6"/>
@@ -1493,6 +1522,7 @@
       <c r="E13" s="4"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
     </row>
     <row r="14" ht="15.35" customHeight="1">
       <c r="A14" s="6"/>
@@ -1502,6 +1532,7 @@
       <c r="E14" s="4"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
     </row>
     <row r="15" ht="15.35" customHeight="1">
       <c r="A15" s="6"/>
@@ -1511,6 +1542,7 @@
       <c r="E15" s="4"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
     </row>
     <row r="16" ht="15.35" customHeight="1">
       <c r="A16" s="6"/>
@@ -1520,6 +1552,7 @@
       <c r="E16" s="4"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
     </row>
     <row r="17" ht="15.35" customHeight="1">
       <c r="A17" s="6"/>
@@ -1529,6 +1562,7 @@
       <c r="E17" s="4"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
     </row>
     <row r="18" ht="15.35" customHeight="1">
       <c r="A18" s="6"/>
@@ -1538,6 +1572,7 @@
       <c r="E18" s="4"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
     </row>
     <row r="19" ht="15.35" customHeight="1">
       <c r="A19" s="6"/>
@@ -1547,6 +1582,7 @@
       <c r="E19" s="4"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
     </row>
     <row r="20" ht="15.35" customHeight="1">
       <c r="A20" s="6"/>
@@ -1556,6 +1592,7 @@
       <c r="E20" s="4"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
     </row>
     <row r="21" ht="15.35" customHeight="1">
       <c r="A21" s="6"/>
@@ -1565,6 +1602,7 @@
       <c r="E21" s="4"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
     </row>
     <row r="22" ht="15.35" customHeight="1">
       <c r="A22" s="6"/>
@@ -1574,6 +1612,7 @@
       <c r="E22" s="4"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
     </row>
     <row r="23" ht="15.35" customHeight="1">
       <c r="A23" s="6"/>
@@ -1583,6 +1622,7 @@
       <c r="E23" s="4"/>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
     </row>
     <row r="24" ht="15.35" customHeight="1">
       <c r="A24" s="6"/>
@@ -1592,6 +1632,7 @@
       <c r="E24" s="4"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
     </row>
     <row r="25" ht="15.35" customHeight="1">
       <c r="A25" s="6"/>
@@ -1601,6 +1642,7 @@
       <c r="E25" s="4"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
     </row>
     <row r="26" ht="15.35" customHeight="1">
       <c r="A26" s="6"/>
@@ -1610,6 +1652,7 @@
       <c r="E26" s="4"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
     </row>
     <row r="27" ht="15.35" customHeight="1">
       <c r="A27" s="6"/>
@@ -1619,6 +1662,7 @@
       <c r="E27" s="4"/>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
     </row>
     <row r="28" ht="15.35" customHeight="1">
       <c r="A28" s="6"/>
@@ -1628,6 +1672,7 @@
       <c r="E28" s="4"/>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
     </row>
     <row r="29" ht="15.35" customHeight="1">
       <c r="A29" s="6"/>
@@ -1637,6 +1682,7 @@
       <c r="E29" s="4"/>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
     </row>
     <row r="30" ht="15.35" customHeight="1">
       <c r="A30" s="6"/>
@@ -1646,6 +1692,7 @@
       <c r="E30" s="4"/>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
     </row>
     <row r="31" ht="15.35" customHeight="1">
       <c r="A31" s="6"/>
@@ -1655,6 +1702,7 @@
       <c r="E31" s="4"/>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
     </row>
     <row r="32" ht="15.35" customHeight="1">
       <c r="A32" s="6"/>
@@ -1664,6 +1712,7 @@
       <c r="E32" s="4"/>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
     </row>
     <row r="33" ht="15.35" customHeight="1">
       <c r="A33" s="6"/>
@@ -1673,6 +1722,7 @@
       <c r="E33" s="4"/>
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
     </row>
     <row r="34" ht="15.35" customHeight="1">
       <c r="A34" s="6"/>
@@ -1682,6 +1732,7 @@
       <c r="E34" s="4"/>
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
     </row>
     <row r="35" ht="15.35" customHeight="1">
       <c r="A35" s="6"/>
@@ -1691,6 +1742,7 @@
       <c r="E35" s="4"/>
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
     </row>
     <row r="36" ht="15.35" customHeight="1">
       <c r="A36" s="6"/>
@@ -1700,6 +1752,7 @@
       <c r="E36" s="4"/>
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
     </row>
     <row r="37" ht="15.35" customHeight="1">
       <c r="A37" s="6"/>
@@ -1709,6 +1762,7 @@
       <c r="E37" s="4"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
     </row>
     <row r="38" ht="15.35" customHeight="1">
       <c r="A38" s="6"/>
@@ -1718,6 +1772,7 @@
       <c r="E38" s="4"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
     </row>
     <row r="39" ht="15.35" customHeight="1">
       <c r="A39" s="6"/>
@@ -1727,6 +1782,7 @@
       <c r="E39" s="4"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
     </row>
     <row r="40" ht="15.35" customHeight="1">
       <c r="A40" s="6"/>
@@ -1736,6 +1792,7 @@
       <c r="E40" s="4"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
     </row>
     <row r="41" ht="15.35" customHeight="1">
       <c r="A41" s="6"/>
@@ -1745,6 +1802,7 @@
       <c r="E41" s="4"/>
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
     </row>
     <row r="42" ht="15.35" customHeight="1">
       <c r="A42" s="6"/>
@@ -1754,6 +1812,7 @@
       <c r="E42" s="4"/>
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
     </row>
     <row r="43" ht="15.35" customHeight="1">
       <c r="A43" s="6"/>
@@ -1763,6 +1822,7 @@
       <c r="E43" s="4"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
     </row>
     <row r="44" ht="15.35" customHeight="1">
       <c r="A44" s="6"/>
@@ -1772,6 +1832,7 @@
       <c r="E44" s="4"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
     </row>
     <row r="45" ht="15.35" customHeight="1">
       <c r="A45" s="6"/>
@@ -1781,6 +1842,7 @@
       <c r="E45" s="4"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
     </row>
     <row r="46" ht="15.35" customHeight="1">
       <c r="A46" s="6"/>
@@ -1790,6 +1852,7 @@
       <c r="E46" s="4"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
     </row>
     <row r="47" ht="15.35" customHeight="1">
       <c r="A47" s="6"/>
@@ -1799,6 +1862,7 @@
       <c r="E47" s="4"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
     </row>
     <row r="48" ht="15.35" customHeight="1">
       <c r="A48" s="6"/>
@@ -1808,6 +1872,7 @@
       <c r="E48" s="4"/>
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
     </row>
     <row r="49" ht="15.35" customHeight="1">
       <c r="A49" s="6"/>
@@ -1817,6 +1882,7 @@
       <c r="E49" s="4"/>
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
     </row>
     <row r="50" ht="15.35" customHeight="1">
       <c r="A50" s="6"/>
@@ -1826,13 +1892,14 @@
       <c r="E50" s="4"/>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
+      <c r="H50" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" location="" tooltip="" display="test@example.com"/>
     <hyperlink ref="F3" r:id="rId2" location="" tooltip="" display="test1@example.com"/>
     <hyperlink ref="F4" r:id="rId3" location="" tooltip="" display="test2@example.com"/>
-    <hyperlink ref="F5" r:id="rId4" location="" tooltip="" display="test@example.com"/>
+    <hyperlink ref="F5" r:id="rId4" location="" tooltip="" display="ttest@example.com"/>
     <hyperlink ref="F6" r:id="rId5" location="" tooltip="" display="test3@example.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511806" footer="0.511806"/>

</xml_diff>